<commit_message>
Trying to prepare the core game logic for a UI
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory/Data/Scenes.xlsx
+++ b/Solution/NeverendingStory/Data/Scenes.xlsx
@@ -1149,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixing text scrolling bug
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory/Data/Scenes.xlsx
+++ b/Solution/NeverendingStory/Data/Scenes.xlsx
@@ -171,9 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">You step very carefully on each stone. Planting your feet solidly on each stone before stepping to the next one, you make it about halfway across the river. Suddenly, a stone that you were stepping on comes loose, careening down the raging river and taking you along with it.
-You get several bruises before you’re able to catch yourself, much further downstream.{if:item:pack: Your pack is swept downstream; your bedroll, all your food, and anything else you had in your pack is gone. You’ll have to forage for food and sleep on the ground from now on.[|REMOVE-pack|][|REMOVE-map|]}
-You drag yourself to the other side of the river. You’re sore all over, and can’t move for hours.
-Once you feel almost ready, you climb back up the river’s edge to the path and continue on your way to {location:goal:namewiththe}.</t>
+You get several bruises before you're able to catch yourself, much further downstream.{if:item:pack: Your pack is swept downstream; your bedroll, all your food, and anything else you had in your pack is gone. You'll have to forage for food and sleep on the ground from now on.[|REMOVE-pack|][|REMOVE-map|]}
+You drag yourself to the other side of the river. You're sore all over, and can't move for hours.
+Once you feel almost ready, you climb back up the river's edge to the path and continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">You climb up the rocks along the river's edge until you find an enormous tree trunk lying across the river. It looks as though someone has recently cut it down. You're able to nimbly walk across the log and cross the river.
@@ -234,7 +234,7 @@
     <t xml:space="preserve">character:baron&amp;baronclaimshometown:true&amp;goal:baronhome&amp;character:ranger&amp;location:current:plains</t>
   </si>
   <si>
-    <t xml:space="preserve">Your path lies through a vast grassland, marked by trees very infrequently. The sun beats down from above, and tall grass obscures your view of the ground you’re walking on.
+    <t xml:space="preserve">Your path lies through a vast grassland, marked by trees very infrequently. The sun beats down from above, and tall grass obscures your view of the ground you're walking on.
 After a day or so, you see a group making its way in your direction, wading through the tall grass. They're getting nearer.</t>
   </si>
   <si>
@@ -244,9 +244,9 @@
     <t xml:space="preserve">Go to meet the group</t>
   </si>
   <si>
-    <t xml:space="preserve">You move to the side and lie down in a particularly dense patch of grass. Hopefully, they’ll pass by you without noticing you. Your head is down, so you can’t see who’s approaching.
+    <t xml:space="preserve">You move to the side and lie down in a particularly dense patch of grass. Hopefully, they'll pass by you without noticing you. Your head is down, so you can't see who's approaching.
 Whoever they are, one of them stumbles just a bit too close to you..
-"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. Now you can see who the group is: two dozen of the {character:baron:baron}’s men in uniform. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
+"What do we have here?" he says. He grabs you roughly by the shoulder and jerks you to your feet. Now you can see who the group is: two dozen of the {character:baron:baron}'s men in uniform. "Well, well, well, the {character:baron:baron} will be THRILLED to meet you!" Cheers erupt.{|BOTW1a|}</t>
   </si>
   <si>
     <t xml:space="preserve">You pick your way towards the group approaching you, being careful to avoid a hidden dip in the terrain. As you get closer, you recognize who they are: two dozen of the {character:baron:baron}'s men in uniform.
@@ -283,7 +283,7 @@
   <si>
     <t xml:space="preserve">{if:location:current:forest:The [location-current-type] is dense here, overgrown and difficult to travel through.}{if:location:current:mountain:The mountain pass is rough here. In many places, you have to climb on all fours to make it over the enormous, jagged rocks.}
 After a day or so, it begins to rain heavily. You take shelter in a nearby cave, making your bed in a small alcove. You go to sleep to wait out the rain.
-When you wake up, you hear something else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It’s still raining outside. They seem to be laying down to sleep. What do you do?</t>
+When you wake up, you hear something else moving in the cave. Opening your eyes, you see two enormous bears, sitting between your alcove and the door. It's still raining outside. They seem to be laying down to sleep. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Try to scare them out of the cave so you can leave</t>
@@ -293,11 +293,11 @@
   </si>
   <si>
     <t xml:space="preserve">You get up suddenly, shouting and waving your arms threateningly.
-The bears are startled at first, but then rear up on their hind legs as well, roaring threateningly. They aren’t backing out, but they do leave you enough room to sneak between them, deftly dodging their sharp claws.
-You make it out{if:noitem:pack: and set off at a run for [location-goal-namewiththe].}{if:item:pack:, but the bears rip your pack off of your back. Your bedroll, all your food, and anything else you had in your pack is gone. You’ll have to forage for food and sleep on the ground from now on.[|REMOVE-pack|][|REMOVE-map|]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It seems like it takes an eternity, but eventually, as it’s getting dark outside again, the two bears settle down, nestled up against each other. You wait until you’re absolutely sure they’re asleep. Then, very, very quietly, you gather your bedroll and sneak past them out of the cave. The rain has stopped by now, and the {location:current:type} is quiet and dark.</t>
+The bears are startled at first, but then rear up on their hind legs as well, roaring threateningly. They aren't backing out, but they do leave you enough room to sneak between them, deftly dodging their sharp claws.
+You make it out{if:noitem:pack: and set off at a run for [location-goal-namewiththe].}{if:item:pack:, but the bears rip your pack off of your back. Your bedroll, all your food, and anything else you had in your pack is gone. You'll have to forage for food and sleep on the ground from now on.[|REMOVE-pack|][|REMOVE-map|]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems like it takes an eternity, but eventually, as it's getting dark outside again, the two bears settle down, nestled up against each other. You wait until you're absolutely sure they're asleep. Then, very, very quietly, you gather your bedroll and sneak past them out of the cave. The rain has stopped by now, and the {location:current:type} is quiet and dark.</t>
   </si>
   <si>
     <t xml:space="preserve">ROT1</t>
@@ -379,13 +379,13 @@
     <t xml:space="preserve">At night, you wonder how your friend {character:taken:name} is right now. It's been a long time since {character:taken:subPronoun} was taken to {location:baronhome:namewiththe} by the {character:baron:baron}'s men.</t>
   </si>
   <si>
-    <t xml:space="preserve">Worry about what’s happened to {character:taken:name}</t>
+    <t xml:space="preserve">Worry about what's happened to {character:taken:name}</t>
   </si>
   <si>
     <t xml:space="preserve">Try to sleep</t>
   </si>
   <si>
-    <t xml:space="preserve">You stay up staring into the fire wondering whether or not {character:taken:name} is safe. It's late before you fall asleep{if:noitem:pack:, lying on the bare ground}. You’re tired the next morning.</t>
+    <t xml:space="preserve">You stay up staring into the fire wondering whether or not {character:taken:name} is safe. It's late before you fall asleep{if:noitem:pack:, lying on the bare ground}. You're tired the next morning.</t>
   </si>
   <si>
     <t xml:space="preserve">You turn over and do your best to fall asleep.{if:noitem:pack: The ground is hard beneath you, with no bedroll.} The next morning comes {if:noitem:pack:slowly}{if:item:pack:quickly}. The sun is rising. You set out for {location:baronhome:namewiththe}, hoping to find {character:taken:name} there.</t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve">location:current:plains&amp;character:mentor</t>
   </si>
   <si>
-    <t xml:space="preserve">You’re in the middle of {location:current:namewiththe}, tall grass as far as the eye can see. The sun is hot, you’re almost out of water, and there’s no shade anywhere. What do you do?</t>
+    <t xml:space="preserve">You're in the middle of {location:current:namewiththe}, tall grass as far as the eye can see. The sun is hot, you're almost out of water, and there's no shade anywhere. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Dismantle your pack to make a small tent for shade</t>
@@ -410,8 +410,8 @@
   </si>
   <si>
     <t xml:space="preserve">You push through the tall grass, your head pounding from dehydration, looking for water anywhere. After a few hours of this, you collapse, unable to move farther.
-Sometime later, you feel someone grabbing your shirt and splashing water in your face. Opening your eyes, you see {pick:character:current:mentor:waterskin}{character:waterskin:name} crouching over you, emptying a waterskin slowly. “You can’t travel in heat like this, you almost died. Here.” {character:waterskin:subPronoun:cap} gives you the waterskin to drink from. You empty it in a few gulps.
-“Carry extra water next time. Take this,” {character:waterskin:name} says, taking the empty waterskin and giving you a full one. “I’ve got a spare.” With that, {character:waterskin:subPronoun} disappears into the grass. {|GIVE:extrawaterskin:[character-waterskin-name]’s waterskin:An extra waterskin [character-waterskin-name] gave you in [location-current-namewiththe]|}</t>
+Sometime later, you feel someone grabbing your shirt and splashing water in your face. Opening your eyes, you see {pick:character:current:mentor:waterskin}{character:waterskin:name} crouching over you, emptying a waterskin slowly. “You can't travel in heat like this, you almost died. Here.” {character:waterskin:subPronoun:cap} gives you the waterskin to drink from. You empty it in a few gulps.
+“Carry extra water next time. Take this,” {character:waterskin:name} says, taking the empty waterskin and giving you a full one. “I've got a spare.” With that, {character:waterskin:subPronoun} disappears into the grass. {|GIVE:extrawaterskin:[character-waterskin-name]'s waterskin:An extra waterskin [character-waterskin-name] gave you in [location-current-namewiththe]|}</t>
   </si>
   <si>
     <t xml:space="preserve">ROT6</t>
@@ -430,8 +430,8 @@
     <t xml:space="preserve">Hold on with all your might</t>
   </si>
   <si>
-    <t xml:space="preserve">Letting go, you slide down the slope, dislodging more rocks as you slide. You hear tremors that threaten an avalanche, but you don’t see one just yet.
-When the skittering stones stop, you resume your climb to the top. You have more ground to make up, but you’re careful not to pull any more stones loose. It’s late when you reach the top.
+    <t xml:space="preserve">Letting go, you slide down the slope, dislodging more rocks as you slide. You hear tremors that threaten an avalanche, but you don't see one just yet.
+When the skittering stones stop, you resume your climb to the top. You have more ground to make up, but you're careful not to pull any more stones loose. It's late when you reach the top.
 You continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
@@ -445,7 +445,7 @@
     <t xml:space="preserve">location:current:swamp</t>
   </si>
   <si>
-    <t xml:space="preserve">You’re wading through murky water in {location:current:namewiththe}. Suddenly, the water around you begins to move. You’re surrounded by crocodiles, each one as long as your outstretched arms. What do you do?</t>
+    <t xml:space="preserve">You're wading through murky water in {location:current:namewiththe}. Suddenly, the water around you begins to move. You're surrounded by crocodiles, each one as long as your outstretched arms. What do you do?</t>
   </si>
   <si>
     <t xml:space="preserve">Fight them off</t>
@@ -455,11 +455,11 @@
   </si>
   <si>
     <t xml:space="preserve">One lunges for you, mouth open. You knock it on the snout with a nearby branch and poke it in the eyes. You scramble madly to shore, waving your branch at any of them that come close to you. One of them bites you in the leg, but a forceful knock between the eyes loosens their grip.
-Your leg is bleeding as you stumble out on to rocky ground. The crocodiles don’t seem to want to follow you there.
+Your leg is bleeding as you stumble out on to rocky ground. The crocodiles don't seem to want to follow you there.
 After putting some distance between yourself and the crocodiles, you wrap up your leg and continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
-    <t xml:space="preserve">You start moving for shore immediately, quickly but without trying to attract attention. One of them starts accelerating toward you as you approach land, its eyes floating above the water as it swims. You scramble madly out of the water and onto rocky ground just before it gets to you. It doesn’t seem to want to follow you there.
+    <t xml:space="preserve">You start moving for shore immediately, quickly but without trying to attract attention. One of them starts accelerating toward you as you approach land, its eyes floating above the water as it swims. You scramble madly out of the water and onto rocky ground just before it gets to you. It doesn't seem to want to follow you there.
 After putting some distance between yourself and the crocodiles, you wrap up your leg and continue on your way to {location:goal:namewiththe}.</t>
   </si>
   <si>
@@ -473,7 +473,7 @@
 Suddenly, an angry badger emerges from a nearby den. It bares it teeth and growls as it approaches, defending its territory against this new intruder.</t>
   </si>
   <si>
-    <t xml:space="preserve">Leave the badger’s territory</t>
+    <t xml:space="preserve">Leave the badger's territory</t>
   </si>
   <si>
     <t xml:space="preserve">Try to pacify it with food</t>
@@ -482,8 +482,8 @@
     <t xml:space="preserve">You back away slowly, returning to the hot sun in {location:current:namewiththe}. Glancing over your shoulder, you can see the badger watching you intently from afar as it disappears below the horizon.</t>
   </si>
   <si>
-    <t xml:space="preserve">Taking your food out of your pack, you toss some on the ground near the badger. Initially, it thinks you’re attacking it, and becomes more aggressive. You back off. Eventually, it realizes you offered it food. You toss it some more. Slowly, it becomes less hostile, and lets you share its copse, but much of your food is gone.
-The shade is a welcome respite from the hot sun. You stay the rest of the day under the watchful eye of the badger. You even manage to catch a few fish in the pond and collect some firewood. Later that day, with night falling, you set out again for {location:goal:namewiththe}, the badger’s gaze disappearing eventually below the horizon.</t>
+    <t xml:space="preserve">Taking your food out of your pack, you toss some on the ground near the badger. Initially, it thinks you're attacking it, and becomes more aggressive. You back off. Eventually, it realizes you offered it food. You toss it some more. Slowly, it becomes less hostile, and lets you share its copse, but much of your food is gone.
+The shade is a welcome respite from the hot sun. You stay the rest of the day under the watchful eye of the badger. You even manage to catch a few fish in the pond and collect some firewood. Later that day, with night falling, you set out again for {location:goal:namewiththe}, the badger's gaze disappearing eventually below the horizon.</t>
   </si>
   <si>
     <t xml:space="preserve">ROT9</t>
@@ -501,8 +501,8 @@
     <t xml:space="preserve">You sit on a nearby stone for a few hours, resting up. After a while, you feel fresh enough to start again. Your legs still feel weaker than usual, but with your newfound strength, you can push on easily toward {location:goal:namewiththe}.</t>
   </si>
   <si>
-    <t xml:space="preserve">Your legs are weak, but through sheer force of will you make them move, over stones and boulders, through trees and brush. You feel like you’ll drop dead from the exertion, but you press on.
-Finally, you see the ground begin to slope down under you. You’ve reached the other side! Your legs regain strength as you hike down {location:current:namewiththe}, toward {location:goal:namewiththe}.</t>
+    <t xml:space="preserve">Your legs are weak, but through sheer force of will you make them move, over stones and boulders, through trees and brush. You feel like you'll drop dead from the exertion, but you press on.
+Finally, you see the ground begin to slope down under you. You've reached the other side! Your legs regain strength as you hike down {location:current:namewiththe}, toward {location:goal:namewiththe}.</t>
   </si>
   <si>
     <t xml:space="preserve">MWG1</t>
@@ -568,11 +568,11 @@
     <t xml:space="preserve">Avoid the camp and push on</t>
   </si>
   <si>
-    <t xml:space="preserve">You turn off the trail, sit down on a stone near the firepit, and finish the half-eaten meal. It’s very good. You wonder what could have made someone abandon their camp up here in {location:current:namewiththe}.
-When you’re done, you rest under the overhang. You still feel sleepy when you wake up, but you set out for {location:goal:namewiththe} anyway, up the mountain pass.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You carry on, avoiding the tempting food. Whoever left the camp surely had a good reason to, and you don’t want to stick around to find out what it was. You press on for {location:goal:namewiththe}, hiking through the mountain pass.</t>
+    <t xml:space="preserve">You turn off the trail, sit down on a stone near the firepit, and finish the half-eaten meal. It's very good. You wonder what could have made someone abandon their camp up here in {location:current:namewiththe}.
+When you're done, you rest under the overhang. You still feel sleepy when you wake up, but you set out for {location:goal:namewiththe} anyway, up the mountain pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You carry on, avoiding the tempting food. Whoever left the camp surely had a good reason to, and you don't want to stick around to find out what it was. You press on for {location:goal:namewiththe}, hiking through the mountain pass.</t>
   </si>
   <si>
     <t xml:space="preserve">AWF1.1</t>
@@ -643,7 +643,7 @@
 You take a few gold coins for yourself from the last chest before you dump it. Just a few, not enough to slow you down.{|GIVE:goldcoins:A few gold coins:from the [character-baron-baron]'s treasury chests|}</t>
   </si>
   <si>
-    <t xml:space="preserve">It takes hours, but you manage to lug each chest of gold outside of {location:current:namewiththe} through {if:item:map:the hidden passage}{if:noitem:map:openings in the guard patrol}. With no shovel, you can’t bury the chests. You want to make sure no one can ever find the gold again.
+    <t xml:space="preserve">It takes hours, but you manage to lug each chest of gold outside of {location:current:namewiththe} through {if:item:map:the hidden passage}{if:noitem:map:openings in the guard patrol}. With no shovel, you can't bury the chests. You want to make sure no one can ever find the gold again.
 Wading into a nearby lake, you open the chests and dump the gold coins as deep into the lake as you can. The lake will pull them under the muck on the bottom, and no one will ever find them. The {character:baron:baron}'s gold is gone.
 You take a few gold coins for yourself from the last chest before you dump it. Just a few, not enough to slow you down.{|GIVE:goldcoins:A few gold coins:from the [character-baron-baron]'s treasury chests|}</t>
   </si>
@@ -738,7 +738,7 @@
     <t xml:space="preserve">MOTW1</t>
   </si>
   <si>
-    <t xml:space="preserve">You {if:noitem:pack:resupply and [|GIVE-pack-Travel pack-food, bedroll, etc.|]}organize a secret meeting at night to rally the people together. They are all ears, ready to hear your plan to rid {location:current:namewiththe} of the {character:baron:baron}’s men. What do you tell them?</t>
+    <t xml:space="preserve">You {if:noitem:pack:resupply and [|GIVE-pack-Travel pack-food, bedroll, etc.|]}organize a secret meeting at night to rally the people together. They are all ears, ready to hear your plan to rid {location:current:namewiththe} of the {character:baron:baron}'s men. What do you tell them?</t>
   </si>
   <si>
     <t xml:space="preserve">Drive them out with force</t>
@@ -750,7 +750,7 @@
     <t xml:space="preserve">You lead the people in a revolt against the {character:baron:baron}'s standing force in {location:current:namewiththe}. Drunk and caught off guard by armed civilians, they're not sure what to do. A few of them are killed before they all retreat, leaving the town forever.</t>
   </si>
   <si>
-    <t xml:space="preserve">That night, the {character:baron:baron}’s men carouse as they always do, demanding food from local businesses they never intend to pay for. But this time, in a coordinated effort by the people of {location:current:namewiththe}, their food and drink is all poisoned. The next morning, not one of the {character:baron:baron}’s men in {location:current:namewiththe} is alive. The people of {location:current:namewiththe} bury them outside of town. They will never bother anyone ever again.</t>
+    <t xml:space="preserve">That night, the {character:baron:baron}'s men carouse as they always do, demanding food from local businesses they never intend to pay for. But this time, in a coordinated effort by the people of {location:current:namewiththe}, their food and drink is all poisoned. The next morning, not one of the {character:baron:baron}'s men in {location:current:namewiththe} is alive. The people of {location:current:namewiththe} bury them outside of town. They will never bother anyone ever again.</t>
   </si>
   <si>
     <t xml:space="preserve">FTL1</t>
@@ -1149,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="7" sqref="C11 C13 C18 C20 C38 D17 D21 F8 F11 F13:G13 F17 F19:F20 F25:G25 G18 G20:G22 G30 G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Improving smooth scrolling in a lot of edge cases
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory/Data/Scenes.xlsx
+++ b/Solution/NeverendingStory/Data/Scenes.xlsx
@@ -50,7 +50,7 @@
   </si>
   <si>
     <t xml:space="preserve">{name}, you live in {location:hometown:name}, a small village {location:hometown:feature:relativeposition}. You work {industry:hometown:workplace} every day, {industry:hometown:goodsGer} enough {industry:hometown:goods} {industry:hometown:purpose} your small village.
-{location:pick:mountain:current:pathtobaron}{location:pick:fortress:pathtobaron:baronhome}{character:pick:baronhome:antagonist:baron}One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {almanac:[character-baron-baron] [character-baron-name]:lays claim to [location-hometown-namewiththe]}{character:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."{|SET:baronclaimshometown:true|}
+{location:pick:forest|swamp|mountain|plains:current:pathtobaron}{location:pick:fortress:pathtobaron:baronhome}{character:pick:baronhome:antagonist:baron}One day, a messenger rides into town. "Citizens of {location:hometown:name}, the {almanac:[character-baron-baron] [character-baron-name]:lays claim to [location-hometown-namewiththe]}{character:baron:baron} {character:baron:name} lays claim to your city. You are now under {character:baron:possPronoun} rule and will pay taxes and fealty to {character:baron:objPronoun}."{|SET:baronclaimshometown:true|}
 What do you do?{character:pick:pathtobaron:mentor:ranger}</t>
   </si>
   <si>
@@ -1149,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="7" sqref="C11 C13 C18 C20 C38 D17 D21 F8 F11 F13:G13 F17 F19:F20 F25:G25 G18 G20:G22 G30 G38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixing title case bug and various Unity-specific bugs, adding some keyboard shortcuts
</commit_message>
<xml_diff>
--- a/Solution/NeverendingStory/Data/Scenes.xlsx
+++ b/Solution/NeverendingStory/Data/Scenes.xlsx
@@ -74,7 +74,7 @@
   <si>
     <t xml:space="preserve">The next week, the {character:baron:baron}'s men arrive. They are soldiers, well-armed and uniformed, with the insignia of the {character:baron:baron} on their jackets.
 They say they're here to collect taxes, but they take so much more than that. They eat food they don't pay for, destroy property that isn't theirs, and leer at young men and women.
-In the morning, your friend {character:pick:hometown:friend:taken}{character:taken:name} is missing. {character:taken:possPronoun:cap} family says that {character:taken:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:baronhome:name}{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}{almanac:[character-baron-baron] [character-baron-name]:lives in [location-baronhome-namewiththe]} by {character:baron:possPronoun} men. They don't know when, or if, {character:taken:subPronoun} will return.{|SET:goal:baronhome|}</t>
+In the morning, your friend {character:pick:hometown:friend:taken}{character:taken:name} is missing.{almanac:[character-taken-name]:your friend from [location-hometown-name], taken to [location-baronhome-name] by the [character-baron-baron]'s men} {character:taken:possPronoun:cap} family says that {character:taken:subPronoun} was taken to {character:baron:baron} {character:baron:name}'s {location:baronhome:name}{almanac:[location-baronhome-namewiththe]:the home of [character-baron-baron] [character-baron-name]}{almanac:[character-baron-baron] [character-baron-name]:lives in [location-baronhome-namewiththe]} by {character:baron:possPronoun} men. They don't know when, or if, {character:taken:subPronoun} will return.{|SET:goal:baronhome|}</t>
   </si>
   <si>
     <t xml:space="preserve">Set out for {location:baronhome:namewiththe} immediately</t>
@@ -709,13 +709,13 @@
     <t xml:space="preserve">Surrender and hope they will spare your life</t>
   </si>
   <si>
-    <t xml:space="preserve">Turn and fight </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You stop in your tracks, put your hands up, and slowly turn around. The {Baron}'s men close the gap between you, slowing to a walk as they approach. {GO TO RFW1.3a}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You turn to face them, {drawing your sword}{readying yourself for battle}. The Baron's men just laugh, drawing their swords and advancing quickly to close the distance. They'll be on you in seconds. {GO TO RFW1.3a}</t>
+    <t xml:space="preserve">Turn and fight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You stop in your tracks, put your hands up, and slowly turn around. The {character:baron:baron}'s men close the gap between you, smiling, slowing to a walk as they approach.{RFW1.3a}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You turn to face them, {if:item:sword:drawing your sword}{if:noitem:sword:readying yourself for a fight}. The Baron's men just laugh, drawing their swords and advancing quickly to close the distance. They'll be on you in seconds.{RFW1.3a}</t>
   </si>
   <si>
     <t xml:space="preserve">RFW1.3a</t>
@@ -1149,8 +1149,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1207,7 +1207,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="191.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>199</v>
       </c>

</xml_diff>